<commit_message>
BOM SU_1000 et SU_11000
pas des spacer car --> triangles
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/SU/SUA1000_SUA1100.xlsx
+++ b/CR - Cost Report/BOM/SU/SUA1000_SUA1100.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\SU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSAE_invictus\STUF2019\CR - Cost Report\BOM\SU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>System</t>
   </si>
@@ -60,18 +60,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
-    <t>m or b</t>
-  </si>
-  <si>
-    <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
-  </si>
-  <si>
     <t>Front uprights</t>
   </si>
   <si>
@@ -122,11 +110,56 @@
   <si>
     <t>SU_A0011</t>
   </si>
+  <si>
+    <t>SU_10005</t>
+  </si>
+  <si>
+    <t>Front Left Upright</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Upper Arm Bracket</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>Upper Arm Wedge Shim</t>
+  </si>
+  <si>
+    <t>Speed Sensor Washer</t>
+  </si>
+  <si>
+    <t>Upper Arm Wedge Base</t>
+  </si>
+  <si>
+    <t>right companion. Al 7075 T6</t>
+  </si>
+  <si>
+    <t>Rear Left Upright</t>
+  </si>
+  <si>
+    <t>2mm, 3mm, 1mm for camber adjustments</t>
+  </si>
+  <si>
+    <t>2mm,3mm, 1mm  for camber adjustments</t>
+  </si>
+  <si>
+    <t>external sensor washer</t>
+  </si>
+  <si>
+    <t>same part as in Front Assembly</t>
+  </si>
+  <si>
+    <t>external sensor washer, same as in Front Assembly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +284,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,26 +562,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="45.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -571,186 +604,204 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
+        <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM SU and bearing preload
to find out
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/SU/SUA1000_SUA1100.xlsx
+++ b/CR - Cost Report/BOM/SU/SUA1000_SUA1100.xlsx
@@ -566,7 +566,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,9 @@
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <v>6</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
@@ -782,7 +784,9 @@
       <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <v>6</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>